<commit_message>
plot Total_PL vs SPY_Return
</commit_message>
<xml_diff>
--- a/09_papers/01_The Unintended Consequences of Rebalancing/backtest_monthly_data_v2.xlsx
+++ b/09_papers/01_The Unintended Consequences of Rebalancing/backtest_monthly_data_v2.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Z279"/>
+  <dimension ref="A1:AA279"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -568,6 +568,11 @@
           <t>Total_PL</t>
         </is>
       </c>
+      <c r="AA1" s="1" t="inlineStr">
+        <is>
+          <t>SPY_Return</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
@@ -648,6 +653,9 @@
       <c r="Z2" t="n">
         <v>0.05658420595089275</v>
       </c>
+      <c r="AA2" t="n">
+        <v>0.01122176035618228</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
@@ -728,6 +736,9 @@
       <c r="Z3" t="n">
         <v>0.05040870305548628</v>
       </c>
+      <c r="AA3" t="n">
+        <v>-0.09633395128199829</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
@@ -808,6 +819,9 @@
       <c r="Z4" t="n">
         <v>0.06719695010182469</v>
       </c>
+      <c r="AA4" t="n">
+        <v>-0.01081832374806435</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
@@ -888,6 +902,9 @@
       <c r="Z5" t="n">
         <v>0.07083709365582602</v>
       </c>
+      <c r="AA5" t="n">
+        <v>0.05119335012537207</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
@@ -968,6 +985,9 @@
       <c r="Z6" t="n">
         <v>0.0653663079358765</v>
       </c>
+      <c r="AA6" t="n">
+        <v>-0.005373868884407496</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
@@ -1048,6 +1068,9 @@
       <c r="Z7" t="n">
         <v>0.1553451129480404</v>
       </c>
+      <c r="AA7" t="n">
+        <v>-0.02802007346142887</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -1128,6 +1151,9 @@
       <c r="Z8" t="n">
         <v>0.1877106694502317</v>
       </c>
+      <c r="AA8" t="n">
+        <v>-0.04036923600372144</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
@@ -1208,6 +1234,9 @@
       <c r="Z9" t="n">
         <v>0.252862874124654</v>
       </c>
+      <c r="AA9" t="n">
+        <v>-0.03535296342496985</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
@@ -1288,6 +1317,9 @@
       <c r="Z10" t="n">
         <v>0.3233598538876579</v>
       </c>
+      <c r="AA10" t="n">
+        <v>0.04741689152505069</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
@@ -1368,6 +1400,9 @@
       <c r="Z11" t="n">
         <v>0.3690251171074724</v>
       </c>
+      <c r="AA11" t="n">
+        <v>0.1018312109101061</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
@@ -1448,6 +1483,9 @@
       <c r="Z12" t="n">
         <v>0.3982577953032215</v>
       </c>
+      <c r="AA12" t="n">
+        <v>0.1133810498872404</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -1528,6 +1566,9 @@
       <c r="Z13" t="n">
         <v>0.4152388426892843</v>
       </c>
+      <c r="AA13" t="n">
+        <v>0.1322781134359047</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
@@ -1608,6 +1649,9 @@
       <c r="Z14" t="n">
         <v>0.3852219409699483</v>
       </c>
+      <c r="AA14" t="n">
+        <v>0.153259682760894</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
@@ -1688,6 +1732,9 @@
       <c r="Z15" t="n">
         <v>0.2991833244069432</v>
       </c>
+      <c r="AA15" t="n">
+        <v>0.1430821972353047</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -1768,6 +1815,9 @@
       <c r="Z16" t="n">
         <v>0.3866769067153299</v>
       </c>
+      <c r="AA16" t="n">
+        <v>0.1958180836958336</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
@@ -1848,6 +1898,9 @@
       <c r="Z17" t="n">
         <v>0.4050572101919566</v>
       </c>
+      <c r="AA17" t="n">
+        <v>0.2071043271390348</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
@@ -1928,6 +1981,9 @@
       <c r="Z18" t="n">
         <v>0.3603015545006283</v>
       </c>
+      <c r="AA18" t="n">
+        <v>0.2566166223421003</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
@@ -2008,6 +2064,9 @@
       <c r="Z19" t="n">
         <v>0.3831524213426786</v>
       </c>
+      <c r="AA19" t="n">
+        <v>0.2766321671139476</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -2088,6 +2147,9 @@
       <c r="Z20" t="n">
         <v>0.3775088298496111</v>
       </c>
+      <c r="AA20" t="n">
+        <v>0.2903756315688453</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
@@ -2168,6 +2230,9 @@
       <c r="Z21" t="n">
         <v>0.4090470725523536</v>
       </c>
+      <c r="AA21" t="n">
+        <v>0.2780439936406425</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
@@ -2248,6 +2313,9 @@
       <c r="Z22" t="n">
         <v>0.4739486111633432</v>
       </c>
+      <c r="AA22" t="n">
+        <v>0.25957608323656</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -2328,6 +2396,9 @@
       <c r="Z23" t="n">
         <v>0.478298862048566</v>
       </c>
+      <c r="AA23" t="n">
+        <v>0.2771194905493898</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -2408,6 +2479,9 @@
       <c r="Z24" t="n">
         <v>0.5184980699753317</v>
       </c>
+      <c r="AA24" t="n">
+        <v>0.2958838776105034</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
@@ -2488,6 +2562,9 @@
       <c r="Z25" t="n">
         <v>0.5669514197023849</v>
       </c>
+      <c r="AA25" t="n">
+        <v>0.2636915243382164</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
@@ -2568,6 +2645,9 @@
       <c r="Z26" t="n">
         <v>0.6203909758064453</v>
       </c>
+      <c r="AA26" t="n">
+        <v>0.2667728047677896</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -2648,6 +2728,9 @@
       <c r="Z27" t="n">
         <v>0.6238033103443182</v>
       </c>
+      <c r="AA27" t="n">
+        <v>0.2770975030248295</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
@@ -2728,6 +2811,9 @@
       <c r="Z28" t="n">
         <v>0.6156836190986242</v>
       </c>
+      <c r="AA28" t="n">
+        <v>0.2905838521166242</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
@@ -2808,6 +2894,9 @@
       <c r="Z29" t="n">
         <v>0.6465111213920472</v>
       </c>
+      <c r="AA29" t="n">
+        <v>0.3345318763807175</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
@@ -2888,6 +2977,9 @@
       <c r="Z30" t="n">
         <v>0.6664719295669593</v>
       </c>
+      <c r="AA30" t="n">
+        <v>0.3644621823245706</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
@@ -2968,6 +3060,9 @@
       <c r="Z31" t="n">
         <v>0.6968776854269719</v>
       </c>
+      <c r="AA31" t="n">
+        <v>0.3421743505856665</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -3048,6 +3143,9 @@
       <c r="Z32" t="n">
         <v>0.6695971489872655</v>
       </c>
+      <c r="AA32" t="n">
+        <v>0.3632908672877427</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
@@ -3128,6 +3226,9 @@
       <c r="Z33" t="n">
         <v>0.652991005589814</v>
       </c>
+      <c r="AA33" t="n">
+        <v>0.3452952053951128</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
@@ -3208,6 +3309,9 @@
       <c r="Z34" t="n">
         <v>0.6171937516698363</v>
       </c>
+      <c r="AA34" t="n">
+        <v>0.3273234410889614</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
@@ -3288,6 +3392,9 @@
       <c r="Z35" t="n">
         <v>0.6537694163748704</v>
       </c>
+      <c r="AA35" t="n">
+        <v>0.359425437794838</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
@@ -3368,6 +3475,9 @@
       <c r="Z36" t="n">
         <v>0.6778565094839084</v>
       </c>
+      <c r="AA36" t="n">
+        <v>0.3612085353974235</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
@@ -3448,6 +3558,9 @@
       <c r="Z37" t="n">
         <v>0.7075660708980601</v>
       </c>
+      <c r="AA37" t="n">
+        <v>0.3990465141195306</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
@@ -3528,6 +3641,9 @@
       <c r="Z38" t="n">
         <v>0.6802652690889915</v>
       </c>
+      <c r="AA38" t="n">
+        <v>0.3900535648781636</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
@@ -3608,6 +3724,9 @@
       <c r="Z39" t="n">
         <v>0.6825476926102535</v>
       </c>
+      <c r="AA39" t="n">
+        <v>0.3983434441535424</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -3688,6 +3807,9 @@
       <c r="Z40" t="n">
         <v>0.745921109856913</v>
       </c>
+      <c r="AA40" t="n">
+        <v>0.375356675025278</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
@@ -3768,6 +3890,9 @@
       <c r="Z41" t="n">
         <v>0.7723596773434911</v>
       </c>
+      <c r="AA41" t="n">
+        <v>0.4186150599725783</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -3848,6 +3973,9 @@
       <c r="Z42" t="n">
         <v>0.8084327701111529</v>
       </c>
+      <c r="AA42" t="n">
+        <v>0.4169259891506677</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -3928,6 +4056,9 @@
       <c r="Z43" t="n">
         <v>0.8226105685360251</v>
       </c>
+      <c r="AA43" t="n">
+        <v>0.4411515347590557</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="n">
@@ -4008,6 +4139,9 @@
       <c r="Z44" t="n">
         <v>0.8112472964434496</v>
       </c>
+      <c r="AA44" t="n">
+        <v>0.4472187841380791</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2" t="n">
@@ -4088,6 +4222,9 @@
       <c r="Z45" t="n">
         <v>0.8154048362885871</v>
       </c>
+      <c r="AA45" t="n">
+        <v>0.4638711557028793</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2" t="n">
@@ -4168,6 +4305,9 @@
       <c r="Z46" t="n">
         <v>0.8141727104620833</v>
       </c>
+      <c r="AA46" t="n">
+        <v>0.4766979977534704</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="n">
@@ -4248,6 +4388,9 @@
       <c r="Z47" t="n">
         <v>0.8160466063121897</v>
       </c>
+      <c r="AA47" t="n">
+        <v>0.4470142173200997</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="n">
@@ -4328,6 +4471,9 @@
       <c r="Z48" t="n">
         <v>0.8651206510996649</v>
       </c>
+      <c r="AA48" t="n">
+        <v>0.4505618109929942</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="n">
@@ -4408,6 +4554,9 @@
       <c r="Z49" t="n">
         <v>0.8797477051203055</v>
       </c>
+      <c r="AA49" t="n">
+        <v>0.4556707034667662</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="n">
@@ -4488,6 +4637,9 @@
       <c r="Z50" t="n">
         <v>0.8823368930129885</v>
       </c>
+      <c r="AA50" t="n">
+        <v>0.4774709760743003</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2" t="n">
@@ -4568,6 +4720,9 @@
       <c r="Z51" t="n">
         <v>0.8994378409578407</v>
       </c>
+      <c r="AA51" t="n">
+        <v>0.5043458634997586</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2" t="n">
@@ -4648,6 +4803,9 @@
       <c r="Z52" t="n">
         <v>0.9375468061988775</v>
       </c>
+      <c r="AA52" t="n">
+        <v>0.5355523820711999</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n">
@@ -4728,6 +4886,9 @@
       <c r="Z53" t="n">
         <v>0.960500707064654</v>
       </c>
+      <c r="AA53" t="n">
+        <v>0.5555620450935556</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="n">
@@ -4808,6 +4969,9 @@
       <c r="Z54" t="n">
         <v>0.9530632929817869</v>
       </c>
+      <c r="AA54" t="n">
+        <v>0.569021674729556</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="n">
@@ -4888,6 +5052,9 @@
       <c r="Z55" t="n">
         <v>0.9392543682948896</v>
       </c>
+      <c r="AA55" t="n">
+        <v>0.5841971415007361</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="n">
@@ -4968,6 +5135,9 @@
       <c r="Z56" t="n">
         <v>0.9949886359548096</v>
       </c>
+      <c r="AA56" t="n">
+        <v>0.5653446087358797</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="n">
@@ -5048,6 +5218,9 @@
       <c r="Z57" t="n">
         <v>0.9711006177172464</v>
       </c>
+      <c r="AA57" t="n">
+        <v>0.5776626508955575</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="n">
@@ -5128,6 +5301,9 @@
       <c r="Z58" t="n">
         <v>0.998745764334753</v>
       </c>
+      <c r="AA58" t="n">
+        <v>0.6212765395112968</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="n">
@@ -5208,6 +5384,9 @@
       <c r="Z59" t="n">
         <v>0.9973799721897769</v>
       </c>
+      <c r="AA59" t="n">
+        <v>0.6549278213883294</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2" t="n">
@@ -5288,6 +5467,9 @@
       <c r="Z60" t="n">
         <v>1.028367133169118</v>
       </c>
+      <c r="AA60" t="n">
+        <v>0.6410610600847755</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2" t="n">
@@ -5368,6 +5550,9 @@
       <c r="Z61" t="n">
         <v>1.134074186556072</v>
       </c>
+      <c r="AA61" t="n">
+        <v>0.6104526130747315</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2" t="n">
@@ -5448,6 +5633,9 @@
       <c r="Z62" t="n">
         <v>1.118856857360085</v>
       </c>
+      <c r="AA62" t="n">
+        <v>0.6254282629860238</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2" t="n">
@@ -5528,6 +5716,9 @@
       <c r="Z63" t="n">
         <v>1.079662128467759</v>
       </c>
+      <c r="AA63" t="n">
+        <v>0.6642242297230614</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2" t="n">
@@ -5608,6 +5799,9 @@
       <c r="Z64" t="n">
         <v>1.09550801740193</v>
       </c>
+      <c r="AA64" t="n">
+        <v>0.6785560433197646</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2" t="n">
@@ -5688,6 +5882,9 @@
       <c r="Z65" t="n">
         <v>1.190856449270118</v>
       </c>
+      <c r="AA65" t="n">
+        <v>0.6418957146731992</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2" t="n">
@@ -5768,6 +5965,9 @@
       <c r="Z66" t="n">
         <v>1.262245276306735</v>
       </c>
+      <c r="AA66" t="n">
+        <v>0.6317988738620132</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2" t="n">
@@ -5848,6 +6048,9 @@
       <c r="Z67" t="n">
         <v>1.368946977920058</v>
       </c>
+      <c r="AA67" t="n">
+        <v>0.5715438059976766</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2" t="n">
@@ -5928,6 +6131,9 @@
       <c r="Z68" t="n">
         <v>1.402467744258102</v>
       </c>
+      <c r="AA68" t="n">
+        <v>0.5466253193246746</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2" t="n">
@@ -6008,6 +6214,9 @@
       <c r="Z69" t="n">
         <v>1.38898730741608</v>
       </c>
+      <c r="AA69" t="n">
+        <v>0.5405325308656875</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2" t="n">
@@ -6088,6 +6297,9 @@
       <c r="Z70" t="n">
         <v>1.436547227995118</v>
       </c>
+      <c r="AA70" t="n">
+        <v>0.5884325533264688</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2" t="n">
@@ -6168,6 +6380,9 @@
       <c r="Z71" t="n">
         <v>1.431544149169</v>
       </c>
+      <c r="AA71" t="n">
+        <v>0.6043338446028715</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2" t="n">
@@ -6248,6 +6463,9 @@
       <c r="Z72" t="n">
         <v>1.413990619186873</v>
       </c>
+      <c r="AA72" t="n">
+        <v>0.5186616188365457</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2" t="n">
@@ -6328,6 +6546,9 @@
       <c r="Z73" t="n">
         <v>1.415825233114734</v>
       </c>
+      <c r="AA73" t="n">
+        <v>0.5116439769943837</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2" t="n">
@@ -6408,6 +6629,9 @@
       <c r="Z74" t="n">
         <v>1.4192058060539</v>
       </c>
+      <c r="AA74" t="n">
+        <v>0.528513567727945</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2" t="n">
@@ -6488,6 +6712,9 @@
       <c r="Z75" t="n">
         <v>1.406923225739583</v>
       </c>
+      <c r="AA75" t="n">
+        <v>0.4391498026503835</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2" t="n">
@@ -6568,6 +6795,9 @@
       <c r="Z76" t="n">
         <v>1.640834338532839</v>
       </c>
+      <c r="AA76" t="n">
+        <v>0.2934456705753445</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2" t="n">
@@ -6648,6 +6878,9 @@
       <c r="Z77" t="n">
         <v>1.788419366896617</v>
       </c>
+      <c r="AA77" t="n">
+        <v>0.2394710121053873</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2" t="n">
@@ -6728,6 +6961,9 @@
       <c r="Z78" t="n">
         <v>1.899197084799209</v>
       </c>
+      <c r="AA78" t="n">
+        <v>0.2582130440115949</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2" t="n">
@@ -6808,6 +7044,9 @@
       <c r="Z79" t="n">
         <v>1.932433607894644</v>
       </c>
+      <c r="AA79" t="n">
+        <v>0.1783942676115644</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2" t="n">
@@ -6888,6 +7127,9 @@
       <c r="Z80" t="n">
         <v>1.892279253275728</v>
       </c>
+      <c r="AA80" t="n">
+        <v>0.06932997523935103</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2" t="n">
@@ -6968,6 +7210,9 @@
       <c r="Z81" t="n">
         <v>1.775547440949747</v>
       </c>
+      <c r="AA81" t="n">
+        <v>0.1589020992314334</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2" t="n">
@@ -7048,6 +7293,9 @@
       <c r="Z82" t="n">
         <v>1.759287199663381</v>
       </c>
+      <c r="AA82" t="n">
+        <v>0.257286163103478</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="2" t="n">
@@ -7128,6 +7376,9 @@
       <c r="Z83" t="n">
         <v>1.789457812715524</v>
       </c>
+      <c r="AA83" t="n">
+        <v>0.3170296777210636</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2" t="n">
@@ -7208,6 +7459,9 @@
       <c r="Z84" t="n">
         <v>1.885978037046394</v>
       </c>
+      <c r="AA84" t="n">
+        <v>0.3180288434173728</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2" t="n">
@@ -7288,6 +7542,9 @@
       <c r="Z85" t="n">
         <v>1.808156419492569</v>
       </c>
+      <c r="AA85" t="n">
+        <v>0.3917421392039608</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2" t="n">
@@ -7368,6 +7625,9 @@
       <c r="Z86" t="n">
         <v>1.910133533927962</v>
       </c>
+      <c r="AA86" t="n">
+        <v>0.4291173749466713</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2" t="n">
@@ -7448,6 +7708,9 @@
       <c r="Z87" t="n">
         <v>1.972529154408344</v>
       </c>
+      <c r="AA87" t="n">
+        <v>0.4648998453103698</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2" t="n">
@@ -7528,6 +7791,9 @@
       <c r="Z88" t="n">
         <v>2.006072858439238</v>
       </c>
+      <c r="AA88" t="n">
+        <v>0.4473766451841837</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="2" t="n">
@@ -7608,6 +7874,9 @@
       <c r="Z89" t="n">
         <v>2.073673508547522</v>
       </c>
+      <c r="AA89" t="n">
+        <v>0.5081250547747965</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2" t="n">
@@ -7688,6 +7957,9 @@
       <c r="Z90" t="n">
         <v>2.100769735223321</v>
       </c>
+      <c r="AA90" t="n">
+        <v>0.5275081427480258</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2" t="n">
@@ -7768,6 +8040,9 @@
       <c r="Z91" t="n">
         <v>2.036573490946509</v>
       </c>
+      <c r="AA91" t="n">
+        <v>0.4915244338502913</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2" t="n">
@@ -7848,6 +8123,9 @@
       <c r="Z92" t="n">
         <v>2.062741784524419</v>
       </c>
+      <c r="AA92" t="n">
+        <v>0.5233674473712387</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="2" t="n">
@@ -7928,6 +8206,9 @@
       <c r="Z93" t="n">
         <v>2.078071463857722</v>
       </c>
+      <c r="AA93" t="n">
+        <v>0.5827898874193351</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2" t="n">
@@ -8008,6 +8289,9 @@
       <c r="Z94" t="n">
         <v>2.134123499945102</v>
       </c>
+      <c r="AA94" t="n">
+        <v>0.5990538129846136</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="2" t="n">
@@ -8088,6 +8372,9 @@
       <c r="Z95" t="n">
         <v>2.262307035331743</v>
       </c>
+      <c r="AA95" t="n">
+        <v>0.5202861854498465</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2" t="n">
@@ -8168,6 +8455,9 @@
       <c r="Z96" t="n">
         <v>2.321957088738943</v>
       </c>
+      <c r="AA96" t="n">
+        <v>0.4699430542244876</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2" t="n">
@@ -8248,6 +8538,9 @@
       <c r="Z97" t="n">
         <v>2.365298851854245</v>
       </c>
+      <c r="AA97" t="n">
+        <v>0.5376529697245216</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2" t="n">
@@ -8328,6 +8621,9 @@
       <c r="Z98" t="n">
         <v>2.300815099519737</v>
       </c>
+      <c r="AA98" t="n">
+        <v>0.4929664289744065</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2" t="n">
@@ -8408,6 +8704,9 @@
       <c r="Z99" t="n">
         <v>2.382215343544257</v>
       </c>
+      <c r="AA99" t="n">
+        <v>0.5798777358659565</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2" t="n">
@@ -8488,6 +8787,9 @@
       <c r="Z100" t="n">
         <v>2.396180888873385</v>
       </c>
+      <c r="AA100" t="n">
+        <v>0.6178256180548314</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2" t="n">
@@ -8568,6 +8870,9 @@
       <c r="Z101" t="n">
         <v>2.486188977352917</v>
       </c>
+      <c r="AA101" t="n">
+        <v>0.6187065355419383</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2" t="n">
@@ -8648,6 +8953,9 @@
       <c r="Z102" t="n">
         <v>2.566954515071068</v>
       </c>
+      <c r="AA102" t="n">
+        <v>0.683818910495443</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="2" t="n">
@@ -8728,6 +9036,9 @@
       <c r="Z103" t="n">
         <v>2.596263359223562</v>
       </c>
+      <c r="AA103" t="n">
+        <v>0.7072595660854032</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2" t="n">
@@ -8808,6 +9119,9 @@
       <c r="Z104" t="n">
         <v>2.646772319444388</v>
       </c>
+      <c r="AA104" t="n">
+        <v>0.7419261917396066</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="2" t="n">
@@ -8888,6 +9202,9 @@
       <c r="Z105" t="n">
         <v>2.669273512841465</v>
       </c>
+      <c r="AA105" t="n">
+        <v>0.7432120621935522</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2" t="n">
@@ -8968,6 +9285,9 @@
       <c r="Z106" t="n">
         <v>2.654406585964969</v>
       </c>
+      <c r="AA106" t="n">
+        <v>0.7720762787061344</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2" t="n">
@@ -9048,6 +9368,9 @@
       <c r="Z107" t="n">
         <v>2.68306170097998</v>
       </c>
+      <c r="AA107" t="n">
+        <v>0.7612591727768013</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2" t="n">
@@ -9128,6 +9451,9 @@
       <c r="Z108" t="n">
         <v>2.770465962030297</v>
       </c>
+      <c r="AA108" t="n">
+        <v>0.7453936644417763</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2" t="n">
@@ -9208,6 +9534,9 @@
       <c r="Z109" t="n">
         <v>2.709870888853954</v>
       </c>
+      <c r="AA109" t="n">
+        <v>0.7261180331998388</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2" t="n">
@@ -9288,6 +9617,9 @@
       <c r="Z110" t="n">
         <v>2.95156033242561</v>
       </c>
+      <c r="AA110" t="n">
+        <v>0.678953434797145</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2" t="n">
@@ -9368,6 +9700,9 @@
       <c r="Z111" t="n">
         <v>3.052774636187309</v>
       </c>
+      <c r="AA111" t="n">
+        <v>0.6104816765638804</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2" t="n">
@@ -9448,6 +9783,9 @@
       <c r="Z112" t="n">
         <v>3.106783476257758</v>
       </c>
+      <c r="AA112" t="n">
+        <v>0.7176455448104427</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2" t="n">
@@ -9528,6 +9866,9 @@
       <c r="Z113" t="n">
         <v>3.177783048426329</v>
       </c>
+      <c r="AA113" t="n">
+        <v>0.7172946369514878</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2" t="n">
@@ -9608,6 +9949,9 @@
       <c r="Z114" t="n">
         <v>3.154424793651259</v>
       </c>
+      <c r="AA114" t="n">
+        <v>0.7290964970783291</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2" t="n">
@@ -9688,6 +10032,9 @@
       <c r="Z115" t="n">
         <v>3.23532612885806</v>
       </c>
+      <c r="AA115" t="n">
+        <v>0.7747654618155794</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2" t="n">
@@ -9768,6 +10115,9 @@
       <c r="Z116" t="n">
         <v>3.296061748312035</v>
       </c>
+      <c r="AA116" t="n">
+        <v>0.8175623868736346</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2" t="n">
@@ -9848,6 +10198,9 @@
       <c r="Z117" t="n">
         <v>3.287913551526663</v>
       </c>
+      <c r="AA117" t="n">
+        <v>0.8497830352610075</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2" t="n">
@@ -9928,6 +10281,9 @@
       <c r="Z118" t="n">
         <v>3.366338060680878</v>
       </c>
+      <c r="AA118" t="n">
+        <v>0.8438683663422469</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2" t="n">
@@ -10008,6 +10364,9 @@
       <c r="Z119" t="n">
         <v>3.362575814314189</v>
       </c>
+      <c r="AA119" t="n">
+        <v>0.7827213671189256</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2" t="n">
@@ -10088,6 +10447,9 @@
       <c r="Z120" t="n">
         <v>3.344101236883968</v>
       </c>
+      <c r="AA120" t="n">
+        <v>0.8242345722185895</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="2" t="n">
@@ -10168,6 +10530,9 @@
       <c r="Z121" t="n">
         <v>3.403271945194724</v>
       </c>
+      <c r="AA121" t="n">
+        <v>0.8367809767732309</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2" t="n">
@@ -10248,6 +10613,9 @@
       <c r="Z122" t="n">
         <v>3.497286808430073</v>
       </c>
+      <c r="AA122" t="n">
+        <v>0.8618841247871257</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2" t="n">
@@ -10328,6 +10696,9 @@
       <c r="Z123" t="n">
         <v>3.564177010602843</v>
       </c>
+      <c r="AA123" t="n">
+        <v>0.8874155766010089</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2" t="n">
@@ -10408,6 +10779,9 @@
       <c r="Z124" t="n">
         <v>3.629684467998578</v>
       </c>
+      <c r="AA124" t="n">
+        <v>0.8695142573955535</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2" t="n">
@@ -10488,6 +10862,9 @@
       <c r="Z125" t="n">
         <v>3.661937442860004</v>
       </c>
+      <c r="AA125" t="n">
+        <v>0.876084623689055</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2" t="n">
@@ -10568,6 +10945,9 @@
       <c r="Z126" t="n">
         <v>3.660687704801466</v>
       </c>
+      <c r="AA126" t="n">
+        <v>0.885485697510784</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2" t="n">
@@ -10648,6 +11028,9 @@
       <c r="Z127" t="n">
         <v>3.673409643893417</v>
       </c>
+      <c r="AA127" t="n">
+        <v>0.9358608131978446</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2" t="n">
@@ -10728,6 +11111,9 @@
       <c r="Z128" t="n">
         <v>3.699393112330283</v>
       </c>
+      <c r="AA128" t="n">
+        <v>0.9491850840648969</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2" t="n">
@@ -10808,6 +11194,9 @@
       <c r="Z129" t="n">
         <v>3.729194570587122</v>
       </c>
+      <c r="AA129" t="n">
+        <v>0.9867062306949702</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2" t="n">
@@ -10888,6 +11277,9 @@
       <c r="Z130" t="n">
         <v>3.808597250618593</v>
       </c>
+      <c r="AA130" t="n">
+        <v>1.006580943476901</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2" t="n">
@@ -10968,6 +11360,9 @@
       <c r="Z131" t="n">
         <v>3.841492790294891</v>
       </c>
+      <c r="AA131" t="n">
+        <v>1.030392622981529</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2" t="n">
@@ -11048,6 +11443,9 @@
       <c r="Z132" t="n">
         <v>3.868719753010387</v>
       </c>
+      <c r="AA132" t="n">
+        <v>1.01810273735165</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="2" t="n">
@@ -11128,6 +11526,9 @@
       <c r="Z133" t="n">
         <v>3.906082671201592</v>
       </c>
+      <c r="AA133" t="n">
+        <v>1.068751808181662</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2" t="n">
@@ -11208,6 +11609,9 @@
       <c r="Z134" t="n">
         <v>3.957238062712689</v>
       </c>
+      <c r="AA134" t="n">
+        <v>1.03877292466042</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2" t="n">
@@ -11288,6 +11692,9 @@
       <c r="Z135" t="n">
         <v>4.024262344617896</v>
       </c>
+      <c r="AA135" t="n">
+        <v>1.070226703955152</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2" t="n">
@@ -11368,6 +11775,9 @@
       <c r="Z136" t="n">
         <v>4.021627153657454</v>
       </c>
+      <c r="AA136" t="n">
+        <v>1.116203946677649</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2" t="n">
@@ -11448,6 +11858,9 @@
       <c r="Z137" t="n">
         <v>4.038178814589445</v>
       </c>
+      <c r="AA137" t="n">
+        <v>1.145727015298041</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2" t="n">
@@ -11528,6 +11941,9 @@
       <c r="Z138" t="n">
         <v>4.012656940472985</v>
       </c>
+      <c r="AA138" t="n">
+        <v>1.171712661637757</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="2" t="n">
@@ -11608,6 +12024,9 @@
       <c r="Z139" t="n">
         <v>3.986878883378274</v>
       </c>
+      <c r="AA139" t="n">
+        <v>1.136492121761004</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2" t="n">
@@ -11688,6 +12107,9 @@
       <c r="Z140" t="n">
         <v>4.01963438766393</v>
       </c>
+      <c r="AA140" t="n">
+        <v>1.1816101418951</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="2" t="n">
@@ -11768,6 +12190,9 @@
       <c r="Z141" t="n">
         <v>4.056307164393612</v>
       </c>
+      <c r="AA141" t="n">
+        <v>1.190274887085558</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2" t="n">
@@ -11848,6 +12273,9 @@
       <c r="Z142" t="n">
         <v>4.068588114876605</v>
       </c>
+      <c r="AA142" t="n">
+        <v>1.197878462342984</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="2" t="n">
@@ -11928,6 +12356,9 @@
       <c r="Z143" t="n">
         <v>4.084392094534879</v>
       </c>
+      <c r="AA143" t="n">
+        <v>1.221089918436599</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2" t="n">
@@ -12008,6 +12439,9 @@
       <c r="Z144" t="n">
         <v>4.134337415472559</v>
       </c>
+      <c r="AA144" t="n">
+        <v>1.241661060006694</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2" t="n">
@@ -12088,6 +12522,9 @@
       <c r="Z145" t="n">
         <v>4.113159930090788</v>
       </c>
+      <c r="AA145" t="n">
+        <v>1.228582508041314</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2" t="n">
@@ -12168,6 +12605,9 @@
       <c r="Z146" t="n">
         <v>4.098690890008135</v>
       </c>
+      <c r="AA146" t="n">
+        <v>1.267559998337485</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2" t="n">
@@ -12248,6 +12688,9 @@
       <c r="Z147" t="n">
         <v>4.147375883615111</v>
       </c>
+      <c r="AA147" t="n">
+        <v>1.254016676436721</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2" t="n">
@@ -12328,6 +12771,9 @@
       <c r="Z148" t="n">
         <v>4.24474270766763</v>
       </c>
+      <c r="AA148" t="n">
+        <v>1.278730109336821</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2" t="n">
@@ -12408,6 +12854,9 @@
       <c r="Z149" t="n">
         <v>4.263613975097651</v>
       </c>
+      <c r="AA149" t="n">
+        <v>1.305915988652709</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2" t="n">
@@ -12488,6 +12937,9 @@
       <c r="Z150" t="n">
         <v>4.243155478677433</v>
       </c>
+      <c r="AA150" t="n">
+        <v>1.304364953963709</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2" t="n">
@@ -12568,6 +13020,9 @@
       <c r="Z151" t="n">
         <v>4.217558907031423</v>
       </c>
+      <c r="AA151" t="n">
+        <v>1.275378791702184</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2" t="n">
@@ -12648,6 +13103,9 @@
       <c r="Z152" t="n">
         <v>4.314621054704379</v>
       </c>
+      <c r="AA152" t="n">
+        <v>1.330452936751879</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2" t="n">
@@ -12728,6 +13186,9 @@
       <c r="Z153" t="n">
         <v>4.27140964608317</v>
       </c>
+      <c r="AA153" t="n">
+        <v>1.315461467997093</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2" t="n">
@@ -12808,6 +13269,9 @@
       <c r="Z154" t="n">
         <v>4.269812732640322</v>
       </c>
+      <c r="AA154" t="n">
+        <v>1.325537907995324</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2" t="n">
@@ -12888,6 +13352,9 @@
       <c r="Z155" t="n">
         <v>4.330448067355563</v>
       </c>
+      <c r="AA155" t="n">
+        <v>1.338748867783982</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2" t="n">
@@ -12968,6 +13435,9 @@
       <c r="Z156" t="n">
         <v>4.374463733737805</v>
       </c>
+      <c r="AA156" t="n">
+        <v>1.31875443630033</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="2" t="n">
@@ -13048,6 +13518,9 @@
       <c r="Z157" t="n">
         <v>4.370200351417227</v>
       </c>
+      <c r="AA157" t="n">
+        <v>1.341669632826013</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2" t="n">
@@ -13128,6 +13601,9 @@
       <c r="Z158" t="n">
         <v>4.440492679614424</v>
       </c>
+      <c r="AA158" t="n">
+        <v>1.281728565556339</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2" t="n">
@@ -13208,6 +13684,9 @@
       <c r="Z159" t="n">
         <v>4.412612036624314</v>
       </c>
+      <c r="AA159" t="n">
+        <v>1.257913158857128</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2" t="n">
@@ -13288,6 +13767,9 @@
       <c r="Z160" t="n">
         <v>4.414951006881738</v>
       </c>
+      <c r="AA160" t="n">
+        <v>1.340356917822078</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2" t="n">
@@ -13368,6 +13850,9 @@
       <c r="Z161" t="n">
         <v>4.465302446337294</v>
       </c>
+      <c r="AA161" t="n">
+        <v>1.344557445249996</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2" t="n">
@@ -13448,6 +13933,9 @@
       <c r="Z162" t="n">
         <v>4.501945832054787</v>
       </c>
+      <c r="AA162" t="n">
+        <v>1.328511757294925</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2" t="n">
@@ -13528,6 +14016,9 @@
       <c r="Z163" t="n">
         <v>4.606948544619433</v>
       </c>
+      <c r="AA163" t="n">
+        <v>1.279572789102752</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="2" t="n">
@@ -13608,6 +14099,9 @@
       <c r="Z164" t="n">
         <v>4.643563695610383</v>
       </c>
+      <c r="AA164" t="n">
+        <v>1.280082525647023</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2" t="n">
@@ -13688,6 +14182,9 @@
       <c r="Z165" t="n">
         <v>4.71171284994917</v>
       </c>
+      <c r="AA165" t="n">
+        <v>1.34580516019536</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2" t="n">
@@ -13768,6 +14265,9 @@
       <c r="Z166" t="n">
         <v>4.703099198156826</v>
       </c>
+      <c r="AA166" t="n">
+        <v>1.350154218147719</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2" t="n">
@@ -13848,6 +14348,9 @@
       <c r="Z167" t="n">
         <v>4.737344366489313</v>
       </c>
+      <c r="AA167" t="n">
+        <v>1.36751029179655</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2" t="n">
@@ -13928,6 +14431,9 @@
       <c r="Z168" t="n">
         <v>4.715240821982057</v>
       </c>
+      <c r="AA168" t="n">
+        <v>1.372430447132581</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2" t="n">
@@ -14008,6 +14514,9 @@
       <c r="Z169" t="n">
         <v>4.715450026592621</v>
       </c>
+      <c r="AA169" t="n">
+        <v>1.408493616139426</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2" t="n">
@@ -14088,6 +14597,9 @@
       <c r="Z170" t="n">
         <v>4.757604350254562</v>
       </c>
+      <c r="AA170" t="n">
+        <v>1.409821605004087</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2" t="n">
@@ -14168,6 +14680,9 @@
       <c r="Z171" t="n">
         <v>4.783915849518115</v>
       </c>
+      <c r="AA171" t="n">
+        <v>1.410682788970535</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="2" t="n">
@@ -14248,6 +14763,9 @@
       <c r="Z172" t="n">
         <v>4.7938849953419</v>
       </c>
+      <c r="AA172" t="n">
+        <v>1.393381451405278</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2" t="n">
@@ -14328,6 +14846,9 @@
       <c r="Z173" t="n">
         <v>4.791357587080006</v>
       </c>
+      <c r="AA173" t="n">
+        <v>1.430025731455393</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="2" t="n">
@@ -14408,6 +14929,9 @@
       <c r="Z174" t="n">
         <v>4.826286978674345</v>
       </c>
+      <c r="AA174" t="n">
+        <v>1.450358473838179</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="2" t="n">
@@ -14488,6 +15012,9 @@
       <c r="Z175" t="n">
         <v>4.815368407385142</v>
       </c>
+      <c r="AA175" t="n">
+        <v>1.468268261402808</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="2" t="n">
@@ -14568,6 +15095,9 @@
       <c r="Z176" t="n">
         <v>4.826289931890197</v>
       </c>
+      <c r="AA176" t="n">
+        <v>1.506921222387008</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="2" t="n">
@@ -14648,6 +15178,9 @@
       <c r="Z177" t="n">
         <v>4.850447210374489</v>
       </c>
+      <c r="AA177" t="n">
+        <v>1.508475671137424</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="2" t="n">
@@ -14728,6 +15261,9 @@
       <c r="Z178" t="n">
         <v>4.863412076861374</v>
       </c>
+      <c r="AA178" t="n">
+        <v>1.518558086513946</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="2" t="n">
@@ -14808,6 +15344,9 @@
       <c r="Z179" t="n">
         <v>4.857521039007691</v>
       </c>
+      <c r="AA179" t="n">
+        <v>1.532824132107936</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2" t="n">
@@ -14888,6 +15427,9 @@
       <c r="Z180" t="n">
         <v>4.869299098564833</v>
       </c>
+      <c r="AA180" t="n">
+        <v>1.539410233110516</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2" t="n">
@@ -14968,6 +15510,9 @@
       <c r="Z181" t="n">
         <v>4.878508207879527</v>
       </c>
+      <c r="AA181" t="n">
+        <v>1.55988392126522</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="2" t="n">
@@ -15048,6 +15593,9 @@
       <c r="Z182" t="n">
         <v>4.895053571206127</v>
       </c>
+      <c r="AA182" t="n">
+        <v>1.563180641953438</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2" t="n">
@@ -15128,6 +15676,9 @@
       <c r="Z183" t="n">
         <v>4.862758023834497</v>
       </c>
+      <c r="AA183" t="n">
+        <v>1.583249654920539</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2" t="n">
@@ -15208,6 +15759,9 @@
       <c r="Z184" t="n">
         <v>4.886347259030401</v>
       </c>
+      <c r="AA184" t="n">
+        <v>1.606657415561507</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="2" t="n">
@@ -15288,6 +15842,9 @@
       <c r="Z185" t="n">
         <v>4.9319800008968</v>
       </c>
+      <c r="AA185" t="n">
+        <v>1.636952568145525</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2" t="n">
@@ -15368,6 +15925,9 @@
       <c r="Z186" t="n">
         <v>4.934621660575636</v>
       </c>
+      <c r="AA186" t="n">
+        <v>1.649125534617237</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="2" t="n">
@@ -15448,6 +16008,9 @@
       <c r="Z187" t="n">
         <v>4.967418294788199</v>
       </c>
+      <c r="AA187" t="n">
+        <v>1.704322490679877</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="2" t="n">
@@ -15528,6 +16091,9 @@
       <c r="Z188" t="n">
         <v>4.956210193675228</v>
       </c>
+      <c r="AA188" t="n">
+        <v>1.670102181089229</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2" t="n">
@@ -15608,6 +16174,9 @@
       <c r="Z189" t="n">
         <v>4.898018326701371</v>
       </c>
+      <c r="AA189" t="n">
+        <v>1.643939055562357</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2" t="n">
@@ -15688,6 +16257,9 @@
       <c r="Z190" t="n">
         <v>4.903092556328263</v>
       </c>
+      <c r="AA190" t="n">
+        <v>1.650258701604213</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2" t="n">
@@ -15768,6 +16340,9 @@
       <c r="Z191" t="n">
         <v>4.954788275730229</v>
       </c>
+      <c r="AA191" t="n">
+        <v>1.674737688215795</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2" t="n">
@@ -15848,6 +16423,9 @@
       <c r="Z192" t="n">
         <v>5.007424557580649</v>
       </c>
+      <c r="AA192" t="n">
+        <v>1.680761938334595</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2" t="n">
@@ -15928,6 +16506,9 @@
       <c r="Z193" t="n">
         <v>5.026879851949941</v>
       </c>
+      <c r="AA193" t="n">
+        <v>1.717451453865074</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="2" t="n">
@@ -16008,6 +16589,9 @@
       <c r="Z194" t="n">
         <v>5.031333624808747</v>
       </c>
+      <c r="AA194" t="n">
+        <v>1.749105141932552</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="2" t="n">
@@ -16088,6 +16672,9 @@
       <c r="Z195" t="n">
         <v>5.038339691888564</v>
       </c>
+      <c r="AA195" t="n">
+        <v>1.755146080938193</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="2" t="n">
@@ -16168,6 +16755,9 @@
       <c r="Z196" t="n">
         <v>4.995553265401406</v>
       </c>
+      <c r="AA196" t="n">
+        <v>1.685790543672034</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="2" t="n">
@@ -16248,6 +16838,9 @@
       <c r="Z197" t="n">
         <v>4.987759401738491</v>
       </c>
+      <c r="AA197" t="n">
+        <v>1.705576373013617</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="2" t="n">
@@ -16328,6 +16921,9 @@
       <c r="Z198" t="n">
         <v>5.126764196280262</v>
       </c>
+      <c r="AA198" t="n">
+        <v>1.616808216103493</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="2" t="n">
@@ -16408,6 +17004,9 @@
       <c r="Z199" t="n">
         <v>5.144247978309938</v>
       </c>
+      <c r="AA199" t="n">
+        <v>1.695286025390874</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="2" t="n">
@@ -16488,6 +17087,9 @@
       <c r="Z200" t="n">
         <v>5.132837856369563</v>
       </c>
+      <c r="AA200" t="n">
+        <v>1.727449271643505</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="2" t="n">
@@ -16568,6 +17170,9 @@
       <c r="Z201" t="n">
         <v>5.121018411489789</v>
       </c>
+      <c r="AA201" t="n">
+        <v>1.745946795327026</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="2" t="n">
@@ -16648,6 +17253,9 @@
       <c r="Z202" t="n">
         <v>5.157411848277929</v>
       </c>
+      <c r="AA202" t="n">
+        <v>1.78617583793178</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="2" t="n">
@@ -16728,6 +17336,9 @@
       <c r="Z203" t="n">
         <v>5.101756988924331</v>
       </c>
+      <c r="AA203" t="n">
+        <v>1.721275384062877</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="2" t="n">
@@ -16808,6 +17419,9 @@
       <c r="Z204" t="n">
         <v>5.158440487643162</v>
       </c>
+      <c r="AA204" t="n">
+        <v>1.789084767299141</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="2" t="n">
@@ -16888,6 +17502,9 @@
       <c r="Z205" t="n">
         <v>5.179578394954683</v>
       </c>
+      <c r="AA205" t="n">
+        <v>1.804396528437638</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="2" t="n">
@@ -16968,6 +17585,9 @@
       <c r="Z206" t="n">
         <v>5.247594307835652</v>
       </c>
+      <c r="AA206" t="n">
+        <v>1.789746670567652</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="2" t="n">
@@ -17048,6 +17668,9 @@
       <c r="Z207" t="n">
         <v>5.306737357564487</v>
       </c>
+      <c r="AA207" t="n">
+        <v>1.809307259758058</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="2" t="n">
@@ -17128,6 +17751,9 @@
       <c r="Z208" t="n">
         <v>5.289446978007605</v>
       </c>
+      <c r="AA208" t="n">
+        <v>1.831907527522093</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="2" t="n">
@@ -17208,6 +17834,9 @@
       <c r="Z209" t="n">
         <v>5.336957800144675</v>
       </c>
+      <c r="AA209" t="n">
+        <v>1.867618051298681</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2" t="n">
@@ -17288,6 +17917,9 @@
       <c r="Z210" t="n">
         <v>5.339523137162546</v>
       </c>
+      <c r="AA210" t="n">
+        <v>1.896502060171657</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2" t="n">
@@ -17368,6 +18000,9 @@
       <c r="Z211" t="n">
         <v>5.275857881363843</v>
       </c>
+      <c r="AA211" t="n">
+        <v>1.896688576705761</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="2" t="n">
@@ -17448,6 +18083,9 @@
       <c r="Z212" t="n">
         <v>5.118823512554368</v>
       </c>
+      <c r="AA212" t="n">
+        <v>1.816656595472595</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="2" t="n">
@@ -17528,6 +18166,9 @@
       <c r="Z213" t="n">
         <v>5.276961244371724</v>
       </c>
+      <c r="AA213" t="n">
+        <v>1.717447693203626</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" s="2" t="n">
@@ -17608,6 +18249,9 @@
       <c r="Z214" t="n">
         <v>5.242243143310477</v>
       </c>
+      <c r="AA214" t="n">
+        <v>1.843757902291388</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" s="2" t="n">
@@ -17688,6 +18332,9 @@
       <c r="Z215" t="n">
         <v>5.197547827984064</v>
       </c>
+      <c r="AA215" t="n">
+        <v>1.892250775572428</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" s="2" t="n">
@@ -17768,6 +18415,9 @@
       <c r="Z216" t="n">
         <v>5.301060180887581</v>
       </c>
+      <c r="AA216" t="n">
+        <v>1.913347088120136</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" s="2" t="n">
@@ -17848,6 +18498,9 @@
       <c r="Z217" t="n">
         <v>5.341141988477786</v>
       </c>
+      <c r="AA217" t="n">
+        <v>1.971353368012489</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" s="2" t="n">
@@ -17928,6 +18581,9 @@
       <c r="Z218" t="n">
         <v>5.317997922884394</v>
       </c>
+      <c r="AA218" t="n">
+        <v>2.039195901888454</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" s="2" t="n">
@@ -18008,6 +18664,9 @@
       <c r="Z219" t="n">
         <v>5.395467657876805</v>
       </c>
+      <c r="AA219" t="n">
+        <v>2.003458242228082</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" s="2" t="n">
@@ -18088,6 +18747,9 @@
       <c r="Z220" t="n">
         <v>5.477420460554968</v>
       </c>
+      <c r="AA220" t="n">
+        <v>1.979960266834802</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="2" t="n">
@@ -18168,6 +18830,9 @@
       <c r="Z221" t="n">
         <v>5.506794036383704</v>
       </c>
+      <c r="AA221" t="n">
+        <v>2.084475537023537</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" s="2" t="n">
@@ -18248,6 +18913,9 @@
       <c r="Z222" t="n">
         <v>5.535100774654787</v>
       </c>
+      <c r="AA222" t="n">
+        <v>2.121193760099986</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" s="2" t="n">
@@ -18328,6 +18996,9 @@
       <c r="Z223" t="n">
         <v>5.62264214769458</v>
       </c>
+      <c r="AA223" t="n">
+        <v>2.111955602321976</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" s="2" t="n">
@@ -18408,6 +19079,9 @@
       <c r="Z224" t="n">
         <v>5.71902274821064</v>
       </c>
+      <c r="AA224" t="n">
+        <v>2.140139495247637</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" s="2" t="n">
@@ -18488,6 +19162,9 @@
       <c r="Z225" t="n">
         <v>5.744455918395061</v>
       </c>
+      <c r="AA225" t="n">
+        <v>2.185740380622205</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" s="2" t="n">
@@ -18568,6 +19245,9 @@
       <c r="Z226" t="n">
         <v>5.729880678584075</v>
       </c>
+      <c r="AA226" t="n">
+        <v>2.237798104020221</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" s="2" t="n">
@@ -18648,6 +19328,9 @@
       <c r="Z227" t="n">
         <v>5.729058402312976</v>
       </c>
+      <c r="AA227" t="n">
+        <v>2.245088470018679</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" s="2" t="n">
@@ -18728,6 +19411,9 @@
       <c r="Z228" t="n">
         <v>5.742369160571331</v>
       </c>
+      <c r="AA228" t="n">
+        <v>2.267586514729649</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" s="2" t="n">
@@ -18808,6 +19494,9 @@
       <c r="Z229" t="n">
         <v>5.773034966300336</v>
       </c>
+      <c r="AA229" t="n">
+        <v>2.292231150394064</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" s="2" t="n">
@@ -18888,6 +19577,9 @@
       <c r="Z230" t="n">
         <v>5.76262142861435</v>
       </c>
+      <c r="AA230" t="n">
+        <v>2.321863010049291</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" s="2" t="n">
@@ -18968,6 +19660,9 @@
       <c r="Z231" t="n">
         <v>5.789638519266845</v>
       </c>
+      <c r="AA231" t="n">
+        <v>2.274840012443133</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" s="2" t="n">
@@ -19048,6 +19743,9 @@
       <c r="Z232" t="n">
         <v>5.843584245210646</v>
       </c>
+      <c r="AA232" t="n">
+        <v>2.343229678444017</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" s="2" t="n">
@@ -19128,6 +19826,9 @@
       <c r="Z233" t="n">
         <v>5.901878820830016</v>
       </c>
+      <c r="AA233" t="n">
+        <v>2.335819974322532</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" s="2" t="n">
@@ -19208,6 +19909,9 @@
       <c r="Z234" t="n">
         <v>5.900663934776589</v>
       </c>
+      <c r="AA234" t="n">
+        <v>2.382266881228192</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" s="2" t="n">
@@ -19288,6 +19992,9 @@
       <c r="Z235" t="n">
         <v>5.90222567444395</v>
       </c>
+      <c r="AA235" t="n">
+        <v>2.329470244494897</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" s="2" t="n">
@@ -19368,6 +20075,9 @@
       <c r="Z236" t="n">
         <v>5.893223083916824</v>
       </c>
+      <c r="AA236" t="n">
+        <v>2.301335205737993</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" s="2" t="n">
@@ -19448,6 +20158,9 @@
       <c r="Z237" t="n">
         <v>5.853638980258047</v>
       </c>
+      <c r="AA237" t="n">
+        <v>2.340643514252467</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" s="2" t="n">
@@ -19528,6 +20241,9 @@
       <c r="Z238" t="n">
         <v>5.916615410111023</v>
       </c>
+      <c r="AA238" t="n">
+        <v>2.251354946562735</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" s="2" t="n">
@@ -19608,6 +20324,9 @@
       <c r="Z239" t="n">
         <v>5.944700010564564</v>
       </c>
+      <c r="AA239" t="n">
+        <v>2.257514440919098</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" s="2" t="n">
@@ -19688,6 +20407,9 @@
       <c r="Z240" t="n">
         <v>5.920611134683707</v>
       </c>
+      <c r="AA240" t="n">
+        <v>2.175144347894155</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" s="2" t="n">
@@ -19768,6 +20490,9 @@
       <c r="Z241" t="n">
         <v>5.917287412978188</v>
       </c>
+      <c r="AA241" t="n">
+        <v>2.2648059588308</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" s="2" t="n">
@@ -19848,6 +20573,9 @@
       <c r="Z242" t="n">
         <v>5.981404736463318</v>
       </c>
+      <c r="AA242" t="n">
+        <v>2.224820803128438</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" s="2" t="n">
@@ -19928,6 +20656,9 @@
       <c r="Z243" t="n">
         <v>6.046502768549672</v>
       </c>
+      <c r="AA243" t="n">
+        <v>2.130332819430893</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" s="2" t="n">
@@ -20008,6 +20739,9 @@
       <c r="Z244" t="n">
         <v>6.074909614987581</v>
       </c>
+      <c r="AA244" t="n">
+        <v>2.21169283642472</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" s="2" t="n">
@@ -20088,6 +20822,9 @@
       <c r="Z245" t="n">
         <v>6.070221569884131</v>
       </c>
+      <c r="AA245" t="n">
+        <v>2.268907508012562</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" s="2" t="n">
@@ -20168,6 +20905,9 @@
       <c r="Z246" t="n">
         <v>6.203945156708896</v>
       </c>
+      <c r="AA246" t="n">
+        <v>2.210924455325149</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" s="2" t="n">
@@ -20248,6 +20988,9 @@
       <c r="Z247" t="n">
         <v>6.266398944281137</v>
       </c>
+      <c r="AA247" t="n">
+        <v>2.273041417885652</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" s="2" t="n">
@@ -20328,6 +21071,9 @@
       <c r="Z248" t="n">
         <v>6.314732836292448</v>
       </c>
+      <c r="AA248" t="n">
+        <v>2.248461091847053</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" s="2" t="n">
@@ -20408,6 +21154,9 @@
       <c r="Z249" t="n">
         <v>6.32524656398395</v>
       </c>
+      <c r="AA249" t="n">
+        <v>2.286334930630454</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" s="2" t="n">
@@ -20488,6 +21237,9 @@
       <c r="Z250" t="n">
         <v>6.321146843919568</v>
       </c>
+      <c r="AA250" t="n">
+        <v>2.302707483901385</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" s="2" t="n">
@@ -20568,6 +21320,9 @@
       <c r="Z251" t="n">
         <v>6.345282585208183</v>
       </c>
+      <c r="AA251" t="n">
+        <v>2.307992643727768</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" s="2" t="n">
@@ -20648,6 +21403,9 @@
       <c r="Z252" t="n">
         <v>6.374766200540637</v>
       </c>
+      <c r="AA252" t="n">
+        <v>2.371310089619948</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" s="2" t="n">
@@ -20728,6 +21486,9 @@
       <c r="Z253" t="n">
         <v>6.379880218658314</v>
       </c>
+      <c r="AA253" t="n">
+        <v>2.403785093581412</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" s="2" t="n">
@@ -20808,6 +21569,9 @@
       <c r="Z254" t="n">
         <v>6.425654038587887</v>
       </c>
+      <c r="AA254" t="n">
+        <v>2.388066659214947</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" s="2" t="n">
@@ -20888,6 +21652,9 @@
       <c r="Z255" t="n">
         <v>6.41207122783615</v>
       </c>
+      <c r="AA255" t="n">
+        <v>2.339980526102556</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" s="2" t="n">
@@ -20968,6 +21735,9 @@
       <c r="Z256" t="n">
         <v>6.46976179024635</v>
       </c>
+      <c r="AA256" t="n">
+        <v>2.318859445155383</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" s="2" t="n">
@@ -21048,6 +21818,9 @@
       <c r="Z257" t="n">
         <v>6.477415908879978</v>
       </c>
+      <c r="AA257" t="n">
+        <v>2.40694595051388</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" s="2" t="n">
@@ -21128,6 +21901,9 @@
       <c r="Z258" t="n">
         <v>6.523059089804148</v>
       </c>
+      <c r="AA258" t="n">
+        <v>2.451978565075654</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" s="2" t="n">
@@ -21208,6 +21984,9 @@
       <c r="Z259" t="n">
         <v>6.571283636733708</v>
       </c>
+      <c r="AA259" t="n">
+        <v>2.468280618240633</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" s="2" t="n">
@@ -21288,6 +22067,9 @@
       <c r="Z260" t="n">
         <v>6.635833559979745</v>
       </c>
+      <c r="AA260" t="n">
+        <v>2.519769365795839</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" s="2" t="n">
@@ -21368,6 +22150,9 @@
       <c r="Z261" t="n">
         <v>6.642473764591875</v>
       </c>
+      <c r="AA261" t="n">
+        <v>2.552330583168034</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" s="2" t="n">
@@ -21448,6 +22233,9 @@
       <c r="Z262" t="n">
         <v>6.640504479045126</v>
       </c>
+      <c r="AA262" t="n">
+        <v>2.511938858285073</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" s="2" t="n">
@@ -21528,6 +22316,9 @@
       <c r="Z263" t="n">
         <v>6.633805814785692</v>
       </c>
+      <c r="AA263" t="n">
+        <v>2.561711090362885</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" s="2" t="n">
@@ -21608,6 +22399,9 @@
       <c r="Z264" t="n">
         <v>6.666533583451297</v>
       </c>
+      <c r="AA264" t="n">
+        <v>2.596560066187129</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" s="2" t="n">
@@ -21688,6 +22482,9 @@
       <c r="Z265" t="n">
         <v>6.702314123045673</v>
       </c>
+      <c r="AA265" t="n">
+        <v>2.609461425007919</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" s="2" t="n">
@@ -21768,6 +22565,9 @@
       <c r="Z266" t="n">
         <v>6.805757469696541</v>
       </c>
+      <c r="AA266" t="n">
+        <v>2.634097319872697</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" s="2" t="n">
@@ -21848,6 +22648,9 @@
       <c r="Z267" t="n">
         <v>6.888478162349321</v>
       </c>
+      <c r="AA267" t="n">
+        <v>2.655597698452503</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" s="2" t="n">
@@ -21928,6 +22731,9 @@
       <c r="Z268" t="n">
         <v>6.936827376108632</v>
       </c>
+      <c r="AA268" t="n">
+        <v>2.647177747586118</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" s="2" t="n">
@@ -22008,6 +22814,9 @@
       <c r="Z269" t="n">
         <v>7.016623229769221</v>
       </c>
+      <c r="AA269" t="n">
+        <v>2.705714067219734</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" s="2" t="n">
@@ -22088,6 +22897,9 @@
       <c r="Z270" t="n">
         <v>7.014693109126116</v>
       </c>
+      <c r="AA270" t="n">
+        <v>2.682194504292216</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" s="2" t="n">
@@ -22168,6 +22980,9 @@
       <c r="Z271" t="n">
         <v>7.051834161600937</v>
       </c>
+      <c r="AA271" t="n">
+        <v>2.709447320796983</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" s="2" t="n">
@@ -22248,6 +23063,9 @@
       <c r="Z272" t="n">
         <v>7.041117374315085</v>
       </c>
+      <c r="AA272" t="n">
+        <v>2.697292396290109</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" s="2" t="n">
@@ -22328,6 +23146,9 @@
       <c r="Z273" t="n">
         <v>7.038163594940666</v>
       </c>
+      <c r="AA273" t="n">
+        <v>2.641745304078706</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" s="2" t="n">
@@ -22408,6 +23229,9 @@
       <c r="Z274" t="n">
         <v>7.148590943537839</v>
       </c>
+      <c r="AA274" t="n">
+        <v>2.643835233376702</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" s="2" t="n">
@@ -22488,6 +23312,9 @@
       <c r="Z275" t="n">
         <v>7.190463387193057</v>
       </c>
+      <c r="AA275" t="n">
+        <v>2.706004286221973</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" s="2" t="n">
@@ -22568,6 +23395,9 @@
       <c r="Z276" t="n">
         <v>7.201670931132824</v>
       </c>
+      <c r="AA276" t="n">
+        <v>2.756549064401958</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" s="2" t="n">
@@ -22648,6 +23478,9 @@
       <c r="Z277" t="n">
         <v>7.227082907593062</v>
       </c>
+      <c r="AA277" t="n">
+        <v>2.779510242625008</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" s="2" t="n">
@@ -22728,6 +23561,9 @@
       <c r="Z278" t="n">
         <v>7.202387276728095</v>
       </c>
+      <c r="AA278" t="n">
+        <v>2.80040005617014</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" s="2" t="n">
@@ -22807,6 +23643,9 @@
       </c>
       <c r="Z279" t="n">
         <v>7.177110474533731</v>
+      </c>
+      <c r="AA279" t="n">
+        <v>2.835634185247261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>